<commit_message>
Somehow failed to save these changes
</commit_message>
<xml_diff>
--- a/PETPEESE_results.xlsx
+++ b/PETPEESE_results.xlsx
@@ -147,11 +147,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,16 +465,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
       <c r="K1" s="1"/>
       <c r="L1" t="s">
         <v>13</v>
@@ -634,7 +634,7 @@
       <c r="L5">
         <v>0.1</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="3">
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="N5">
@@ -669,7 +669,7 @@
       <c r="L6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="3">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="N6">
@@ -704,7 +704,7 @@
       <c r="L7">
         <v>0.11</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="3">
         <v>2.3E-2</v>
       </c>
       <c r="N7">
@@ -727,7 +727,7 @@
       <c r="E8">
         <v>0.12</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>4.99E-2</v>
       </c>
       <c r="G8">
@@ -748,7 +748,7 @@
       <c r="L8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="N8">
@@ -774,7 +774,7 @@
       <c r="E9">
         <v>0.31</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G9">
@@ -809,7 +809,7 @@
       <c r="E10">
         <v>0.16</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G10">
@@ -867,7 +867,7 @@
       <c r="E12">
         <v>0.21</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>1E-3</v>
       </c>
       <c r="G12">
@@ -890,7 +890,7 @@
       <c r="E13">
         <v>0.21</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="G13">
@@ -925,7 +925,7 @@
       <c r="E14">
         <v>0.16</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G14">
@@ -945,7 +945,7 @@
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor edits to script and output
</commit_message>
<xml_diff>
--- a/PETPEESE_results.xlsx
+++ b/PETPEESE_results.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-330" yWindow="3225" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
   <si>
     <t>Outcome</t>
   </si>
@@ -92,12 +92,27 @@
   <si>
     <t>is this including Panee &amp; Ballard nonsense?</t>
   </si>
+  <si>
+    <t>Craig</t>
+  </si>
+  <si>
+    <t>r+</t>
+  </si>
+  <si>
+    <t>Reproduce</t>
+  </si>
+  <si>
+    <t>Getting different results in reproduction for AggCog cross-sectional b/c of exclusion of Matsuzaki.</t>
+  </si>
+  <si>
+    <t>Must be some experimental effect sizes still showing up on several rows for AggBeh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,13 +157,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -241,7 +259,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -276,7 +293,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -452,38 +468,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E1" s="4" t="s">
+    <row r="1" spans="1:21">
+      <c r="E1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="1"/>
-      <c r="L1" t="s">
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="1"/>
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -497,13 +520,13 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
         <v>3</v>
@@ -515,16 +538,16 @@
         <v>6</v>
       </c>
       <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" t="s">
         <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" t="s">
-        <v>6</v>
       </c>
       <c r="O2" t="s">
         <v>3</v>
@@ -535,8 +558,17 @@
       <c r="Q2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -550,28 +582,37 @@
         <v>21</v>
       </c>
       <c r="E3">
+        <v>21</v>
+      </c>
+      <c r="F3">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="G3">
+        <v>0.31</v>
+      </c>
+      <c r="H3">
         <v>-0.12</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>0.27100000000000002</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>12</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>20</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>-0.03</v>
       </c>
-      <c r="M3">
+      <c r="P3">
         <v>0.68100000000000005</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -585,28 +626,37 @@
         <v>37</v>
       </c>
       <c r="E4">
+        <v>37</v>
+      </c>
+      <c r="F4">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="G4">
+        <v>0.19</v>
+      </c>
+      <c r="H4">
         <v>-0.13</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <v>0.154</v>
       </c>
-      <c r="G4">
+      <c r="J4">
         <v>1E-3</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>36</v>
       </c>
-      <c r="L4">
+      <c r="O4">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="M4">
+      <c r="P4">
         <v>0.33200000000000002</v>
       </c>
-      <c r="N4">
+      <c r="Q4">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -620,28 +670,37 @@
         <v>12</v>
       </c>
       <c r="E5">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G5">
+        <v>0.11</v>
+      </c>
+      <c r="H5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>0.16200000000000001</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <v>0.32400000000000001</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>11</v>
       </c>
-      <c r="L5">
+      <c r="O5">
         <v>0.1</v>
       </c>
-      <c r="M5" s="3">
+      <c r="P5" s="3">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="N5">
+      <c r="Q5">
         <v>0.60199999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -655,28 +714,37 @@
         <v>20</v>
       </c>
       <c r="E6">
+        <v>19</v>
+      </c>
+      <c r="F6">
+        <v>0.11</v>
+      </c>
+      <c r="G6">
+        <v>0.15</v>
+      </c>
+      <c r="H6">
         <v>0.12</v>
       </c>
-      <c r="F6">
+      <c r="I6">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="G6">
+      <c r="J6">
         <v>0.59799999999999998</v>
       </c>
-      <c r="K6">
+      <c r="N6">
         <v>18</v>
       </c>
-      <c r="L6">
+      <c r="O6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M6" s="3">
+      <c r="P6" s="3">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="N6">
+      <c r="Q6">
         <v>0.14099999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -690,28 +758,37 @@
         <v>29</v>
       </c>
       <c r="E7">
+        <v>27</v>
+      </c>
+      <c r="F7">
+        <v>0.21</v>
+      </c>
+      <c r="G7">
+        <v>0.22</v>
+      </c>
+      <c r="H7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F7">
+      <c r="I7">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="G7" t="s">
+      <c r="J7" t="s">
         <v>12</v>
       </c>
-      <c r="K7">
+      <c r="N7">
         <v>28</v>
       </c>
-      <c r="L7">
+      <c r="O7">
         <v>0.11</v>
       </c>
-      <c r="M7" s="3">
+      <c r="P7" s="3">
         <v>2.3E-2</v>
       </c>
-      <c r="N7">
+      <c r="Q7">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -725,40 +802,49 @@
         <v>47</v>
       </c>
       <c r="E8">
+        <v>45</v>
+      </c>
+      <c r="F8">
+        <v>0.18</v>
+      </c>
+      <c r="G8">
+        <v>0.19</v>
+      </c>
+      <c r="H8">
         <v>0.12</v>
       </c>
-      <c r="F8" s="3">
+      <c r="I8" s="3">
         <v>4.99E-2</v>
-      </c>
-      <c r="G8">
-        <v>0.187</v>
-      </c>
-      <c r="H8">
-        <v>0.16</v>
-      </c>
-      <c r="I8" t="s">
-        <v>12</v>
       </c>
       <c r="J8">
         <v>0.187</v>
       </c>
       <c r="K8">
+        <v>0.16</v>
+      </c>
+      <c r="L8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8">
+        <v>0.187</v>
+      </c>
+      <c r="N8">
         <v>46</v>
       </c>
-      <c r="L8">
+      <c r="O8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M8" s="3">
+      <c r="P8" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="N8">
+      <c r="Q8">
         <v>0.35499999999999998</v>
       </c>
-      <c r="R8" t="s">
+      <c r="U8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -772,28 +858,37 @@
         <v>44</v>
       </c>
       <c r="E9">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.26</v>
+      </c>
+      <c r="H9">
         <v>0.31</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G9">
+      <c r="J9">
         <v>0.48699999999999999</v>
       </c>
-      <c r="K9">
+      <c r="N9">
         <v>43</v>
       </c>
-      <c r="L9">
+      <c r="O9">
         <v>0.27</v>
       </c>
-      <c r="M9" t="s">
+      <c r="P9" t="s">
         <v>12</v>
       </c>
-      <c r="N9">
+      <c r="Q9">
         <v>0.71599999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -807,28 +902,37 @@
         <v>84</v>
       </c>
       <c r="E10">
+        <v>81</v>
+      </c>
+      <c r="F10">
+        <v>0.189</v>
+      </c>
+      <c r="G10">
+        <v>0.18</v>
+      </c>
+      <c r="H10">
         <v>0.16</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G10">
+      <c r="J10">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="K10">
+      <c r="N10">
         <v>81</v>
       </c>
-      <c r="L10">
+      <c r="O10">
         <v>0.16</v>
       </c>
-      <c r="M10" t="s">
+      <c r="P10" t="s">
         <v>12</v>
       </c>
-      <c r="N10">
+      <c r="Q10">
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -842,16 +946,25 @@
         <v>24</v>
       </c>
       <c r="E11">
+        <v>24</v>
+      </c>
+      <c r="F11">
+        <v>0.217</v>
+      </c>
+      <c r="G11">
+        <v>0.22</v>
+      </c>
+      <c r="H11">
         <v>0.11</v>
       </c>
-      <c r="F11">
+      <c r="I11">
         <v>0.16500000000000001</v>
       </c>
-      <c r="G11">
+      <c r="J11">
         <v>0.123</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -865,16 +978,25 @@
         <v>48</v>
       </c>
       <c r="E12">
+        <v>48</v>
+      </c>
+      <c r="F12">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="G12">
         <v>0.21</v>
       </c>
-      <c r="F12" s="3">
+      <c r="H12">
+        <v>0.21</v>
+      </c>
+      <c r="I12" s="3">
         <v>1E-3</v>
       </c>
-      <c r="G12">
+      <c r="J12">
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -888,28 +1010,37 @@
         <v>27</v>
       </c>
       <c r="E13">
+        <v>27</v>
+      </c>
+      <c r="F13">
+        <v>0.183</v>
+      </c>
+      <c r="G13">
+        <v>0.16</v>
+      </c>
+      <c r="H13">
         <v>0.21</v>
       </c>
-      <c r="F13" s="3">
+      <c r="I13" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G13">
+      <c r="J13">
         <v>0.89200000000000002</v>
       </c>
-      <c r="K13">
+      <c r="N13">
         <v>25</v>
       </c>
-      <c r="L13">
+      <c r="O13">
         <v>0.08</v>
       </c>
-      <c r="M13">
+      <c r="P13">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="N13">
+      <c r="Q13">
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -923,36 +1054,56 @@
         <v>38</v>
       </c>
       <c r="E14">
+        <v>38</v>
+      </c>
+      <c r="F14">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="G14">
+        <v>0.15</v>
+      </c>
+      <c r="H14">
         <v>0.16</v>
       </c>
-      <c r="F14" s="3">
+      <c r="I14" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G14">
+      <c r="J14">
         <v>0.78300000000000003</v>
       </c>
-      <c r="K14">
+      <c r="N14">
         <v>36</v>
       </c>
-      <c r="L14">
+      <c r="O14">
         <v>0.15</v>
       </c>
-      <c r="M14">
+      <c r="P14">
         <v>1E-3</v>
       </c>
-      <c r="N14">
+      <c r="Q14">
         <v>0.79300000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="E1:G1"/>
+  <mergeCells count="3">
     <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -960,24 +1111,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>